<commit_message>
Casos club y metodos
</commit_message>
<xml_diff>
--- a/LineasClubPersonalFront.xlsx
+++ b/LineasClubPersonalFront.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Telecom\WebPersonal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A674155\eclipse-workspace\WebPersonal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E36C7B3-E9CD-4331-8D0F-82BB5FF0A060}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{510C4170-454D-432F-9C2F-96A292DDDE87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Linea</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>Resumen_de_Puntos_PRE</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Credito_MIX</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Credito_PRE</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Pack_MIX</t>
+  </si>
+  <si>
+    <t>Canje_de_Puntos_Canje_de_Pack_PRE</t>
   </si>
 </sst>
 </file>
@@ -427,13 +439,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -577,6 +589,38 @@
         <v>1162676705</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>1162676705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1162816939</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1162676705</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>